<commit_message>
Added DDM valuation and README addition
</commit_message>
<xml_diff>
--- a/BHP.xlsx
+++ b/BHP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konstantin/Documents/valuations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C979FC-9420-B848-B311-0390A421CC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC38668E-7CD9-BB4C-80B2-CD0F5E839AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="880" windowWidth="36000" windowHeight="22500" tabRatio="767" activeTab="6" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" tabRatio="767" activeTab="6" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="162">
   <si>
     <t>Font</t>
   </si>
@@ -544,18 +544,71 @@
   <si>
     <t>No volume growth in the last 10 years. Assumption therefore also 0%</t>
   </si>
+  <si>
+    <t>FY24-29E</t>
+  </si>
+  <si>
+    <t>2% increases yoy from FY24</t>
+  </si>
+  <si>
+    <t>Retention of earnings</t>
+  </si>
+  <si>
+    <t>Distributable profits</t>
+  </si>
+  <si>
+    <t>No retention needed, TV growth retention</t>
+  </si>
+  <si>
+    <t>Discount rate</t>
+  </si>
+  <si>
+    <t>Risk free rate</t>
+  </si>
+  <si>
+    <t>Market risk premium</t>
+  </si>
+  <si>
+    <t>Betafactor</t>
+  </si>
+  <si>
+    <t>yfinance (5Y monthly)</t>
+  </si>
+  <si>
+    <t>Rough</t>
+  </si>
+  <si>
+    <t>Risk premium</t>
+  </si>
+  <si>
+    <t>Discount factor</t>
+  </si>
+  <si>
+    <t>Valuation date</t>
+  </si>
+  <si>
+    <t>Country risk premium</t>
+  </si>
+  <si>
+    <t>Present values</t>
+  </si>
+  <si>
+    <t>Sum of present values</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%;\(0.0%\)"/>
     <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="168" formatCode="#,###.0\x"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.00%;\(0.00%\)"/>
+    <numFmt numFmtId="173" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -832,7 +885,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -923,7 +976,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -957,6 +1009,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1669,10 +1733,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" zoomScale="133" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1748,188 +1812,176 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="67">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E14" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B15" s="5" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B16" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>2025</v>
       </c>
-      <c r="G15">
-        <f>+F15+1</f>
+      <c r="G16">
+        <f>+F16+1</f>
         <v>2026</v>
       </c>
-      <c r="H15">
-        <f t="shared" ref="H15:J15" si="0">+G15+1</f>
+      <c r="H16">
+        <f t="shared" ref="H16:J16" si="0">+G16+1</f>
         <v>2027</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="K15" s="59" t="s">
+      <c r="K16" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="53">
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="52">
         <v>0.01</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B19" s="5" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B20" s="5" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B20" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="57">
-        <v>10000</v>
-      </c>
-      <c r="G20" s="57">
-        <f>F20+250</f>
-        <v>10250</v>
-      </c>
-      <c r="H20" s="57">
-        <f t="shared" ref="H20:J20" si="1">G20+250</f>
-        <v>10500</v>
-      </c>
-      <c r="I20" s="57">
-        <f t="shared" si="1"/>
-        <v>10750</v>
-      </c>
-      <c r="J20" s="57">
-        <f t="shared" si="1"/>
-        <v>11000</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="57">
-        <f>AVERAGE(Model!K43:O43)+5</f>
-        <v>128.66274683848124</v>
-      </c>
-      <c r="G21" s="57">
-        <f>AVERAGE(Model!L43:P43)+5</f>
-        <v>132.78099755193318</v>
-      </c>
-      <c r="H21" s="57">
-        <f>AVERAGE(Model!M43:Q43)+5</f>
-        <v>127.70486343984962</v>
-      </c>
-      <c r="I21" s="57">
-        <f>AVERAGE(Model!N43:R43)+5</f>
-        <v>129.10506318095966</v>
-      </c>
-      <c r="J21" s="57">
-        <f>AVERAGE(Model!O43:S43)+5</f>
-        <v>130.86301241919688</v>
+        <v>128</v>
+      </c>
+      <c r="E21" s="51"/>
+      <c r="F21" s="56">
+        <f>Model!O42*1.02</f>
+        <v>9324.9435912262397</v>
+      </c>
+      <c r="G21" s="56">
+        <f>F21*1.02</f>
+        <v>9511.4424630507656</v>
+      </c>
+      <c r="H21" s="56">
+        <f t="shared" ref="H21:J21" si="1">G21*1.02</f>
+        <v>9701.6713123117806</v>
+      </c>
+      <c r="I21" s="56">
+        <f t="shared" si="1"/>
+        <v>9895.7047385580172</v>
+      </c>
+      <c r="J21" s="56">
+        <f t="shared" si="1"/>
+        <v>10093.618833329178</v>
+      </c>
+      <c r="M21" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="51"/>
+      <c r="F22" s="56">
+        <f>Model!O43*1.02</f>
+        <v>113.28261890645587</v>
+      </c>
+      <c r="G22" s="56">
+        <f>F22*1.02</f>
+        <v>115.54827128458498</v>
+      </c>
+      <c r="H22" s="56">
+        <f t="shared" ref="H22:J22" si="2">G22*1.02</f>
+        <v>117.85923671027669</v>
+      </c>
+      <c r="I22" s="56">
+        <f t="shared" si="2"/>
+        <v>120.21642144448222</v>
+      </c>
+      <c r="J22" s="56">
+        <f t="shared" si="2"/>
+        <v>122.62074987337186</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="57">
-        <f>AVERAGE(Model!K44:O44)+5</f>
-        <v>189.36832828486422</v>
-      </c>
-      <c r="G22" s="57">
-        <f>AVERAGE(Model!L44:P44)+5</f>
-        <v>214.84535431950698</v>
-      </c>
-      <c r="H22" s="57">
-        <f>AVERAGE(Model!M44:Q44)+5</f>
-        <v>229.01747630632798</v>
-      </c>
-      <c r="I22" s="57">
-        <f>AVERAGE(Model!N44:R44)+5</f>
-        <v>197.98702491648615</v>
-      </c>
-      <c r="J22" s="57">
-        <f>AVERAGE(Model!O44:S44)+5</f>
-        <v>199.95391312598164</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B24" s="5" t="s">
+      <c r="E23" s="51"/>
+      <c r="F23" s="56">
+        <f>Model!O44*1.02</f>
+        <v>146.42240943877738</v>
+      </c>
+      <c r="G23" s="56">
+        <f>F23*1.02</f>
+        <v>149.35085762755293</v>
+      </c>
+      <c r="H23" s="56">
+        <f t="shared" ref="H23:J23" si="3">G23*1.02</f>
+        <v>152.33787478010399</v>
+      </c>
+      <c r="I23" s="56">
+        <f t="shared" si="3"/>
+        <v>155.38463227570608</v>
+      </c>
+      <c r="J23" s="56">
+        <f t="shared" si="3"/>
+        <v>158.49232492122022</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B25" s="5" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="62">
-        <v>0</v>
-      </c>
-      <c r="G25" s="62">
-        <v>0</v>
-      </c>
-      <c r="H25" s="62">
-        <v>0</v>
-      </c>
-      <c r="I25" s="62">
-        <v>0</v>
-      </c>
-      <c r="J25" s="62">
-        <v>0</v>
-      </c>
-      <c r="M25" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="62">
+        <v>88</v>
+      </c>
+      <c r="E26" s="51"/>
+      <c r="F26" s="61">
         <v>0</v>
       </c>
-      <c r="G26" s="62">
+      <c r="G26" s="61">
         <v>0</v>
       </c>
-      <c r="H26" s="62">
+      <c r="H26" s="61">
         <v>0</v>
       </c>
-      <c r="I26" s="62">
+      <c r="I26" s="61">
         <v>0</v>
       </c>
-      <c r="J26" s="62">
+      <c r="J26" s="61">
         <v>0</v>
       </c>
       <c r="M26" t="s">
@@ -1938,22 +1990,22 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="62">
+        <v>93</v>
+      </c>
+      <c r="E27" s="51"/>
+      <c r="F27" s="61">
         <v>0</v>
       </c>
-      <c r="G27" s="62">
+      <c r="G27" s="61">
         <v>0</v>
       </c>
-      <c r="H27" s="62">
+      <c r="H27" s="61">
         <v>0</v>
       </c>
-      <c r="I27" s="62">
+      <c r="I27" s="61">
         <v>0</v>
       </c>
-      <c r="J27" s="62">
+      <c r="J27" s="61">
         <v>0</v>
       </c>
       <c r="M27" t="s">
@@ -1961,75 +2013,145 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="63"/>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="51"/>
+      <c r="F28" s="61">
+        <v>0</v>
+      </c>
+      <c r="G28" s="61">
+        <v>0</v>
+      </c>
+      <c r="H28" s="61">
+        <v>0</v>
+      </c>
+      <c r="I28" s="61">
+        <v>0</v>
+      </c>
+      <c r="J28" s="61">
+        <v>0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B29" t="s">
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B30" t="s">
         <v>142</v>
       </c>
-      <c r="E29" s="52"/>
-      <c r="F29" s="62">
+      <c r="E30" s="51"/>
+      <c r="F30" s="61">
         <f>MEDIAN(Model!K25:O25)</f>
         <v>0.42596642386174915</v>
       </c>
-      <c r="G29" s="62">
-        <f>F29</f>
+      <c r="G30" s="61">
+        <f>F30</f>
         <v>0.42596642386174915</v>
       </c>
-      <c r="H29" s="62">
-        <f t="shared" ref="H29:J29" si="2">G29</f>
+      <c r="H30" s="61">
+        <f t="shared" ref="H30:J30" si="4">G30</f>
         <v>0.42596642386174915</v>
       </c>
-      <c r="I29" s="62">
-        <f t="shared" si="2"/>
+      <c r="I30" s="61">
+        <f t="shared" si="4"/>
         <v>0.42596642386174915</v>
       </c>
-      <c r="J29" s="62">
-        <f t="shared" si="2"/>
+      <c r="J30" s="61">
+        <f t="shared" si="4"/>
         <v>0.42596642386174915</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M30" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="63"/>
-    </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B31" t="s">
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B32" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="52"/>
-      <c r="F31" s="62">
+      <c r="E32" s="51"/>
+      <c r="F32" s="61">
         <f>MEDIAN(Model!K26:O26)</f>
         <v>0.35336787564766842</v>
       </c>
-      <c r="G31" s="62">
-        <f>F31</f>
+      <c r="G32" s="61">
+        <f>F32</f>
         <v>0.35336787564766842</v>
       </c>
-      <c r="H31" s="62">
-        <f t="shared" ref="H31:J31" si="3">G31</f>
+      <c r="H32" s="61">
+        <f t="shared" ref="H32:J32" si="5">G32</f>
         <v>0.35336787564766842</v>
       </c>
-      <c r="I31" s="62">
-        <f t="shared" si="3"/>
+      <c r="I32" s="61">
+        <f t="shared" si="5"/>
         <v>0.35336787564766842</v>
       </c>
-      <c r="J31" s="62">
-        <f t="shared" si="3"/>
+      <c r="J32" s="61">
+        <f t="shared" si="5"/>
         <v>0.35336787564766842</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M32" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B34" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="63">
+        <v>0.04</v>
+      </c>
+      <c r="M35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="63">
+        <v>0.04</v>
+      </c>
+      <c r="M36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0.78</v>
+      </c>
+      <c r="M37" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>159</v>
+      </c>
+      <c r="E38" s="63">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2061,8 +2183,8 @@
   </sheetPr>
   <dimension ref="A1:P704"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="183" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="183" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
@@ -2110,7 +2232,7 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.15">
       <c r="E9" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F9" s="37"/>
@@ -2272,51 +2394,70 @@
       <c r="P18" s="18"/>
     </row>
     <row r="19" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
+      <c r="E19" s="5" t="str">
+        <f>Input!$E$8&amp;" - DDM valuation"</f>
+        <v>BHP - DDM valuation</v>
+      </c>
+      <c r="P19" s="9"/>
     </row>
     <row r="20" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="E20" s="10" t="str">
+        <f>+Input!$E$14</f>
+        <v>USDmn</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="J20" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="K20" s="47" t="s">
+        <v>126</v>
+      </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
       <c r="P20" s="18"/>
     </row>
-    <row r="21" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-    </row>
+    <row r="21" spans="5:16" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="22" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
+      <c r="E22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="19">
+        <f>Model!P22</f>
+        <v>14706.455549117749</v>
+      </c>
+      <c r="G22" s="19">
+        <f>Model!Q22</f>
+        <v>15015.379729758721</v>
+      </c>
+      <c r="H22" s="19">
+        <f>Model!R22</f>
+        <v>15330.437777662466</v>
+      </c>
+      <c r="I22" s="19">
+        <f>Model!S22</f>
+        <v>15651.751924010734</v>
+      </c>
+      <c r="J22" s="19">
+        <f>Model!T22</f>
+        <v>15979.446840147291</v>
+      </c>
+      <c r="K22" s="19">
+        <f>Model!U22</f>
+        <v>16148.869660880368</v>
+      </c>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
@@ -2324,116 +2465,297 @@
       <c r="P22" s="18"/>
     </row>
     <row r="23" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
+      <c r="E23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" s="18">
+        <v>0</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0</v>
+      </c>
+      <c r="H23" s="18">
+        <v>0</v>
+      </c>
+      <c r="I23" s="18">
+        <v>0</v>
+      </c>
+      <c r="J23" s="18">
+        <v>0</v>
+      </c>
+      <c r="K23" s="18">
+        <f>Historical!O48*Model!B3*-1</f>
+        <v>-491.2</v>
+      </c>
       <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
+      <c r="M23" s="18" t="s">
+        <v>149</v>
+      </c>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
       <c r="P23" s="18"/>
     </row>
     <row r="24" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
+      <c r="E24" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="64">
+        <f>SUM(F22:F23)</f>
+        <v>14706.455549117749</v>
+      </c>
+      <c r="G24" s="64">
+        <f t="shared" ref="G24:K24" si="0">SUM(G22:G23)</f>
+        <v>15015.379729758721</v>
+      </c>
+      <c r="H24" s="64">
+        <f t="shared" si="0"/>
+        <v>15330.437777662466</v>
+      </c>
+      <c r="I24" s="64">
+        <f t="shared" si="0"/>
+        <v>15651.751924010734</v>
+      </c>
+      <c r="J24" s="64">
+        <f t="shared" si="0"/>
+        <v>15979.446840147291</v>
+      </c>
+      <c r="K24" s="64">
+        <f t="shared" si="0"/>
+        <v>15657.669660880367</v>
+      </c>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
     </row>
-    <row r="25" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
+    <row r="25" spans="5:16" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="E25" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="66">
+        <f>Input!$E$35</f>
+        <v>0.04</v>
+      </c>
+      <c r="G25" s="66">
+        <f>F25</f>
+        <v>0.04</v>
+      </c>
+      <c r="H25" s="66">
+        <f t="shared" ref="H25:K25" si="1">G25</f>
+        <v>0.04</v>
+      </c>
+      <c r="I25" s="66">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="J25" s="66">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="K25" s="66">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
       <c r="P25" s="18"/>
     </row>
-    <row r="26" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
+    <row r="26" spans="5:16" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="E26" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="68">
+        <f>Input!E37</f>
+        <v>0.78</v>
+      </c>
+      <c r="G26" s="68">
+        <f>F26</f>
+        <v>0.78</v>
+      </c>
+      <c r="H26" s="68">
+        <f t="shared" ref="H26:K26" si="2">G26</f>
+        <v>0.78</v>
+      </c>
+      <c r="I26" s="68">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+      <c r="J26" s="68">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+      <c r="K26" s="68">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
       <c r="P26" s="18"/>
     </row>
-    <row r="27" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
+    <row r="27" spans="5:16" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="E27" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="66">
+        <f>Input!E36</f>
+        <v>0.04</v>
+      </c>
+      <c r="G27" s="66">
+        <f>F27</f>
+        <v>0.04</v>
+      </c>
+      <c r="H27" s="66">
+        <f t="shared" ref="H27:K27" si="3">G27</f>
+        <v>0.04</v>
+      </c>
+      <c r="I27" s="66">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="J27" s="66">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="K27" s="66">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
       <c r="L27" s="18"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
       <c r="O27" s="18"/>
       <c r="P27" s="18"/>
     </row>
-    <row r="28" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
+    <row r="28" spans="5:16" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="E28" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="F28" s="66">
+        <f>Input!E38</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="66">
+        <f t="shared" ref="G28:K28" si="4">F28</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="66">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
       <c r="P28" s="18"/>
     </row>
-    <row r="29" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
+    <row r="29" spans="5:16" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="E29" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" s="66">
+        <f>F26*F27+F28</f>
+        <v>3.1200000000000002E-2</v>
+      </c>
+      <c r="G29" s="66">
+        <f t="shared" ref="G29:K29" si="5">G26*G27+G28</f>
+        <v>3.1200000000000002E-2</v>
+      </c>
+      <c r="H29" s="66">
+        <f t="shared" si="5"/>
+        <v>3.1200000000000002E-2</v>
+      </c>
+      <c r="I29" s="66">
+        <f t="shared" si="5"/>
+        <v>3.1200000000000002E-2</v>
+      </c>
+      <c r="J29" s="66">
+        <f t="shared" si="5"/>
+        <v>3.1200000000000002E-2</v>
+      </c>
+      <c r="K29" s="66">
+        <f t="shared" si="5"/>
+        <v>3.1200000000000002E-2</v>
+      </c>
+      <c r="L29" s="66"/>
       <c r="M29" s="18"/>
       <c r="N29" s="18"/>
       <c r="O29" s="18"/>
       <c r="P29" s="18"/>
     </row>
-    <row r="30" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
+    <row r="30" spans="5:16" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="E30" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="66">
+        <v>0</v>
+      </c>
+      <c r="G30" s="66">
+        <v>0</v>
+      </c>
+      <c r="H30" s="66">
+        <v>0</v>
+      </c>
+      <c r="I30" s="66">
+        <v>0</v>
+      </c>
+      <c r="J30" s="66">
+        <v>0</v>
+      </c>
+      <c r="K30" s="66">
+        <f>Input!K18*-1</f>
+        <v>-0.01</v>
+      </c>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
       <c r="O30" s="18"/>
       <c r="P30" s="18"/>
     </row>
-    <row r="31" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
+    <row r="31" spans="5:16" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="E31" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="66">
+        <f>F29+F25+F30</f>
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="G31" s="66">
+        <f t="shared" ref="G31:K31" si="6">G29+G25+G30</f>
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="H31" s="66">
+        <f t="shared" si="6"/>
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="I31" s="66">
+        <f t="shared" si="6"/>
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="J31" s="66">
+        <f t="shared" si="6"/>
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="K31" s="66">
+        <f t="shared" si="6"/>
+        <v>6.1199999999999997E-2</v>
+      </c>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
@@ -2441,33 +2763,81 @@
       <c r="P31" s="18"/>
     </row>
     <row r="32" spans="5:16" x14ac:dyDescent="0.15">
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
+      <c r="E32" s="65" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="68">
+        <f>1/(1+F31)^1</f>
+        <v>0.93353248693054525</v>
+      </c>
+      <c r="G32" s="68">
+        <f>F32/(1+G31)^1</f>
+        <v>0.87148290415472862</v>
+      </c>
+      <c r="H32" s="68">
+        <f t="shared" ref="H32:J32" si="7">G32/(1+H31)^1</f>
+        <v>0.81355760283301781</v>
+      </c>
+      <c r="I32" s="68">
+        <f t="shared" si="7"/>
+        <v>0.75948245223395994</v>
+      </c>
+      <c r="J32" s="68">
+        <f t="shared" si="7"/>
+        <v>0.70900154241407765</v>
+      </c>
+      <c r="K32" s="68">
+        <f>J32/K31</f>
+        <v>11.584992523105845</v>
+      </c>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
       <c r="N32" s="18"/>
       <c r="O32" s="18"/>
       <c r="P32" s="18"/>
     </row>
-    <row r="33" spans="6:16" x14ac:dyDescent="0.15">
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
+    <row r="33" spans="5:16" x14ac:dyDescent="0.15">
+      <c r="E33" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F33" s="19">
+        <f>F24*F32</f>
+        <v>13728.954022701409</v>
+      </c>
+      <c r="G33" s="19">
+        <f t="shared" ref="G33:K33" si="8">G24*G32</f>
+        <v>13085.646733876174</v>
+      </c>
+      <c r="H33" s="19">
+        <f t="shared" si="8"/>
+        <v>12472.194208775813</v>
+      </c>
+      <c r="I33" s="19">
+        <f t="shared" si="8"/>
+        <v>11887.230933005272</v>
+      </c>
+      <c r="J33" s="19">
+        <f t="shared" si="8"/>
+        <v>11329.452456588189</v>
+      </c>
+      <c r="K33" s="19">
+        <f t="shared" si="8"/>
+        <v>181393.98595056028</v>
+      </c>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
       <c r="O33" s="18"/>
       <c r="P33" s="18"/>
     </row>
-    <row r="34" spans="6:16" x14ac:dyDescent="0.15">
-      <c r="F34" s="18"/>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.15">
+      <c r="E34" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="19">
+        <f>SUM(F33:K33)</f>
+        <v>243897.46430550714</v>
+      </c>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
@@ -2479,7 +2849,7 @@
       <c r="O34" s="18"/>
       <c r="P34" s="18"/>
     </row>
-    <row r="35" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2492,7 +2862,7 @@
       <c r="O35" s="18"/>
       <c r="P35" s="18"/>
     </row>
-    <row r="36" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="36" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
@@ -2505,7 +2875,7 @@
       <c r="O36" s="18"/>
       <c r="P36" s="18"/>
     </row>
-    <row r="37" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="37" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
@@ -2518,7 +2888,7 @@
       <c r="O37" s="18"/>
       <c r="P37" s="18"/>
     </row>
-    <row r="38" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
@@ -2531,7 +2901,7 @@
       <c r="O38" s="18"/>
       <c r="P38" s="18"/>
     </row>
-    <row r="39" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
@@ -2544,7 +2914,7 @@
       <c r="O39" s="18"/>
       <c r="P39" s="18"/>
     </row>
-    <row r="40" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
@@ -2557,7 +2927,7 @@
       <c r="O40" s="18"/>
       <c r="P40" s="18"/>
     </row>
-    <row r="41" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
@@ -2570,7 +2940,7 @@
       <c r="O41" s="18"/>
       <c r="P41" s="18"/>
     </row>
-    <row r="42" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="42" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
       <c r="H42" s="18"/>
@@ -2583,7 +2953,7 @@
       <c r="O42" s="18"/>
       <c r="P42" s="18"/>
     </row>
-    <row r="43" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="43" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
@@ -2596,7 +2966,7 @@
       <c r="O43" s="18"/>
       <c r="P43" s="18"/>
     </row>
-    <row r="44" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="44" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -2609,7 +2979,7 @@
       <c r="O44" s="18"/>
       <c r="P44" s="18"/>
     </row>
-    <row r="45" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="45" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
@@ -2622,7 +2992,7 @@
       <c r="O45" s="18"/>
       <c r="P45" s="18"/>
     </row>
-    <row r="46" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="46" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F46" s="18"/>
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
@@ -2635,7 +3005,7 @@
       <c r="O46" s="18"/>
       <c r="P46" s="18"/>
     </row>
-    <row r="47" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="47" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
@@ -2648,7 +3018,7 @@
       <c r="O47" s="18"/>
       <c r="P47" s="18"/>
     </row>
-    <row r="48" spans="6:16" x14ac:dyDescent="0.15">
+    <row r="48" spans="5:16" x14ac:dyDescent="0.15">
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -11205,10 +11575,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:Z747"/>
+  <dimension ref="A1:AA747"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="119" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
@@ -11216,26 +11586,26 @@
     <col min="1" max="3" width="9.1640625" style="8" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="2.33203125" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="52.83203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="52.83203125" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:27" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="B1" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="B2" s="17" t="e">
         <f>AND(C:C)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="56">
-        <f>Input!$K$17</f>
+      <c r="B3" s="55">
+        <f>Input!$K$18</f>
         <v>0.01</v>
       </c>
       <c r="D3" s="5" t="str">
@@ -11243,19 +11613,19 @@
         <v>Model</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="D4" s="6" t="str">
         <f>Cover!$A$2</f>
         <v>Indicative valuation of BHP Group Limited: Public information</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
       <c r="D5" s="6" t="str">
         <f>Cover!$A$3</f>
         <v>Educational purposes only, no financial advice</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E8" s="5" t="str">
         <f>Input!$E$8&amp;" P&amp;L"</f>
         <v>BHP P&amp;L</v>
@@ -11271,13 +11641,14 @@
         <v>111</v>
       </c>
       <c r="X8" s="39"/>
-      <c r="Z8" s="36" t="s">
+      <c r="Y8" s="39"/>
+      <c r="AA8" s="36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E9" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F9" s="37" t="s">
@@ -11334,9 +11705,12 @@
       <c r="X9" s="39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="Y9" s="39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E11" s="13" t="s">
         <v>27</v>
       </c>
@@ -11372,27 +11746,27 @@
       </c>
       <c r="P11" s="18">
         <f>P39</f>
-        <v>64538.649610401881</v>
+        <v>56887.479999999996</v>
       </c>
       <c r="Q11" s="18">
         <f t="shared" ref="Q11:U11" si="0">Q39</f>
-        <v>67460.733441756005</v>
+        <v>58009.031600000002</v>
       </c>
       <c r="R11" s="18">
         <f t="shared" si="0"/>
-        <v>67465.232426946226</v>
+        <v>59152.852252000004</v>
       </c>
       <c r="S11" s="18">
         <f t="shared" si="0"/>
-        <v>66685.944870984633</v>
+        <v>60319.385717239995</v>
       </c>
       <c r="T11" s="18">
         <f t="shared" si="0"/>
-        <v>67759.01280984495</v>
+        <v>61509.084615986802</v>
       </c>
       <c r="U11" s="18">
         <f t="shared" si="0"/>
-        <v>68436.602937943404</v>
+        <v>62124.175462146668</v>
       </c>
       <c r="W11" s="29">
         <f>IFERROR((O11/F11)^(1/9)-1,"n/a")</f>
@@ -11402,8 +11776,12 @@
         <f>IFERROR((O11/L11)^(1/3)-1,"n/a")</f>
         <v>-2.9115574512328934E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="Y11" s="29">
+        <f>IFERROR((T11/O11)^(1/5)-1,"n/a")</f>
+        <v>2.0192986291499571E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
@@ -11437,12 +11815,12 @@
       <c r="O12" s="18">
         <v>1285</v>
       </c>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
       <c r="W12" s="29">
         <f t="shared" ref="W12:W22" si="1">IFERROR((O12/F12)^(1/9)-1,"n/a")</f>
         <v>0.11156718365981</v>
@@ -11451,8 +11829,12 @@
         <f t="shared" ref="X12:X22" si="2">IFERROR((O12/L12)^(1/3)-1,"n/a")</f>
         <v>0.36074783033775892</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="Y12" s="29">
+        <f t="shared" ref="Y12:Y22" si="3">IFERROR((T12/O12)^(1/5)-1,"n/a")</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E13" s="13" t="s">
         <v>29</v>
       </c>
@@ -11486,12 +11868,12 @@
       <c r="O13" s="18">
         <v>-36750</v>
       </c>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="52"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="51"/>
       <c r="W13" s="29">
         <f t="shared" si="1"/>
         <v>-7.8301780801481868E-4</v>
@@ -11500,8 +11882,12 @@
         <f t="shared" si="2"/>
         <v>2.1282952880393058E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="Y13" s="29">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E14" s="13" t="s">
         <v>30</v>
       </c>
@@ -11535,12 +11921,12 @@
       <c r="O14" s="20">
         <v>-2656</v>
       </c>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="58"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
       <c r="W14" s="29">
         <f>IFERROR((O14/F14)^(1/9)-1,"n/a")</f>
         <v>-2.1916832490021325</v>
@@ -11549,74 +11935,78 @@
         <f t="shared" si="2"/>
         <v>0.42338640502534819</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="Y14" s="29">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E15" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="19">
-        <f t="shared" ref="F15:O15" si="3">SUM(F11:F14)</f>
+        <f t="shared" ref="F15:O15" si="4">SUM(F11:F14)</f>
         <v>8670</v>
       </c>
       <c r="G15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2804</v>
       </c>
       <c r="H15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12554</v>
       </c>
       <c r="I15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15996</v>
       </c>
       <c r="J15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16113</v>
       </c>
       <c r="K15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14421</v>
       </c>
       <c r="L15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25906</v>
       </c>
       <c r="M15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34106</v>
       </c>
       <c r="N15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22932</v>
       </c>
       <c r="O15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17537</v>
       </c>
       <c r="P15" s="19">
         <f>P11*P25</f>
-        <v>27491.297775409359</v>
+        <v>24232.156418106777</v>
       </c>
       <c r="Q15" s="19">
-        <f t="shared" ref="Q15:U15" si="4">Q11*Q25</f>
-        <v>28736.007375275516</v>
+        <f t="shared" ref="Q15:U15" si="5">Q11*Q25</f>
+        <v>24709.899742335201</v>
       </c>
       <c r="R15" s="19">
-        <f t="shared" si="4"/>
-        <v>28737.923791908001</v>
+        <f t="shared" si="5"/>
+        <v>25197.128935006858</v>
       </c>
       <c r="S15" s="19">
-        <f t="shared" si="4"/>
-        <v>28405.973458535078</v>
+        <f t="shared" si="5"/>
+        <v>25694.03302351019</v>
       </c>
       <c r="T15" s="19">
-        <f t="shared" si="4"/>
-        <v>28863.064371012104</v>
+        <f t="shared" si="5"/>
+        <v>26200.804808881629</v>
       </c>
       <c r="U15" s="19">
-        <f t="shared" si="4"/>
-        <v>29151.695014722227</v>
+        <f t="shared" si="5"/>
+        <v>26462.812856970442</v>
       </c>
       <c r="W15" s="41">
         <f t="shared" si="1"/>
@@ -11626,8 +12016,12 @@
         <f t="shared" si="2"/>
         <v>-0.12195188761232589</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="Y15" s="41">
+        <f t="shared" si="3"/>
+        <v>8.3607159880387361E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
       <c r="E16" s="16" t="s">
         <v>31</v>
       </c>
@@ -11661,12 +12055,12 @@
       <c r="O16" s="18">
         <v>-2198</v>
       </c>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="52"/>
-      <c r="R16" s="52"/>
-      <c r="S16" s="52"/>
-      <c r="T16" s="52"/>
-      <c r="U16" s="52"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="51"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="51"/>
+      <c r="U16" s="51"/>
       <c r="W16" s="29">
         <f t="shared" si="1"/>
         <v>0.13521136582617932</v>
@@ -11675,8 +12069,12 @@
         <f t="shared" si="2"/>
         <v>0.16840343073730279</v>
       </c>
-    </row>
-    <row r="17" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y16" s="29">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E17" s="16" t="s">
         <v>32</v>
       </c>
@@ -11710,12 +12108,12 @@
       <c r="O17" s="20">
         <v>709</v>
       </c>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="52"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
       <c r="W17" s="29">
         <f t="shared" si="1"/>
         <v>0.26091218130279215</v>
@@ -11724,45 +12122,49 @@
         <f t="shared" si="2"/>
         <v>1.1335743996040399</v>
       </c>
-    </row>
-    <row r="18" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y17" s="29">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E18" s="14" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="22">
-        <f t="shared" ref="F18:N18" si="5">SUM(F16:F17)</f>
+        <f t="shared" ref="F18:N18" si="6">SUM(F16:F17)</f>
         <v>-614</v>
       </c>
       <c r="G18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1013</v>
       </c>
       <c r="H18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1417</v>
       </c>
       <c r="I18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1245</v>
       </c>
       <c r="J18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1064</v>
       </c>
       <c r="K18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-911</v>
       </c>
       <c r="L18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1305</v>
       </c>
       <c r="M18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-969</v>
       </c>
       <c r="N18" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1531</v>
       </c>
       <c r="O18" s="22">
@@ -11774,23 +12176,23 @@
         <v>-1489</v>
       </c>
       <c r="Q18" s="22">
-        <f t="shared" ref="Q18:U18" si="6">P18</f>
+        <f t="shared" ref="Q18:U18" si="7">P18</f>
         <v>-1489</v>
       </c>
       <c r="R18" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1489</v>
       </c>
       <c r="S18" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1489</v>
       </c>
       <c r="T18" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1489</v>
       </c>
       <c r="U18" s="22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1489</v>
       </c>
       <c r="W18" s="41">
@@ -11801,45 +12203,49 @@
         <f t="shared" si="2"/>
         <v>4.4948119363673822E-2</v>
       </c>
-    </row>
-    <row r="19" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y18" s="41">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E19" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F19" s="19">
-        <f t="shared" ref="F19:N19" si="7">+F15+F18</f>
+        <f t="shared" ref="F19:N19" si="8">+F15+F18</f>
         <v>8056</v>
       </c>
       <c r="G19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1791</v>
       </c>
       <c r="H19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11137</v>
       </c>
       <c r="I19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14751</v>
       </c>
       <c r="J19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15049</v>
       </c>
       <c r="K19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13510</v>
       </c>
       <c r="L19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24601</v>
       </c>
       <c r="M19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>33137</v>
       </c>
       <c r="N19" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21401</v>
       </c>
       <c r="O19" s="19">
@@ -11847,28 +12253,28 @@
         <v>16048</v>
       </c>
       <c r="P19" s="19">
-        <f t="shared" ref="P19:U19" si="8">+P15+P18</f>
-        <v>26002.297775409359</v>
+        <f t="shared" ref="P19:U19" si="9">+P15+P18</f>
+        <v>22743.156418106777</v>
       </c>
       <c r="Q19" s="19">
-        <f t="shared" si="8"/>
-        <v>27247.007375275516</v>
+        <f t="shared" si="9"/>
+        <v>23220.899742335201</v>
       </c>
       <c r="R19" s="19">
-        <f t="shared" si="8"/>
-        <v>27248.923791908001</v>
+        <f t="shared" si="9"/>
+        <v>23708.128935006858</v>
       </c>
       <c r="S19" s="19">
-        <f t="shared" si="8"/>
-        <v>26916.973458535078</v>
+        <f t="shared" si="9"/>
+        <v>24205.03302351019</v>
       </c>
       <c r="T19" s="19">
-        <f t="shared" si="8"/>
-        <v>27374.064371012104</v>
+        <f t="shared" si="9"/>
+        <v>24711.804808881629</v>
       </c>
       <c r="U19" s="19">
-        <f t="shared" si="8"/>
-        <v>27662.695014722227</v>
+        <f t="shared" si="9"/>
+        <v>24973.812856970442</v>
       </c>
       <c r="W19" s="41">
         <f t="shared" si="1"/>
@@ -11878,8 +12284,12 @@
         <f t="shared" si="2"/>
         <v>-0.13272654979285703</v>
       </c>
-    </row>
-    <row r="20" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y19" s="41">
+        <f t="shared" si="3"/>
+        <v>9.0176233351402679E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E20" t="s">
         <v>36</v>
       </c>
@@ -11915,27 +12325,27 @@
       </c>
       <c r="P20" s="18">
         <f>P19*P26*-1</f>
-        <v>-9188.3767268544998</v>
+        <v>-8036.7008689890272</v>
       </c>
       <c r="Q20" s="18">
-        <f t="shared" ref="Q20:U20" si="9">Q19*Q26*-1</f>
-        <v>-9628.2171139574621</v>
+        <f t="shared" ref="Q20:U20" si="10">Q19*Q26*-1</f>
+        <v>-8205.5200125764804</v>
       </c>
       <c r="R20" s="18">
-        <f t="shared" si="9"/>
-        <v>-9628.8943140317406</v>
+        <f t="shared" si="10"/>
+        <v>-8377.6911573443922</v>
       </c>
       <c r="S20" s="18">
-        <f t="shared" si="9"/>
-        <v>-9511.5937299072139</v>
+        <f t="shared" si="10"/>
+        <v>-8553.2810994994561</v>
       </c>
       <c r="T20" s="18">
-        <f t="shared" si="9"/>
-        <v>-9673.1149746270748</v>
+        <f t="shared" si="10"/>
+        <v>-8732.3579687343372</v>
       </c>
       <c r="U20" s="18">
-        <f t="shared" si="9"/>
-        <v>-9775.1077720417416</v>
+        <f t="shared" si="10"/>
+        <v>-8824.9431960900747</v>
       </c>
       <c r="W20" s="29">
         <f t="shared" si="1"/>
@@ -11945,8 +12355,12 @@
         <f t="shared" si="2"/>
         <v>-0.16690549943429955</v>
       </c>
-    </row>
-    <row r="21" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y20" s="29">
+        <f t="shared" si="3"/>
+        <v>6.2563203094661235E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E21" t="s">
         <v>105</v>
       </c>
@@ -12006,74 +12420,78 @@
         <f t="shared" si="2"/>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="22" spans="5:24" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="Y21" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="22" spans="5:25" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="E22" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="23">
-        <f t="shared" ref="F22:U22" si="10">SUM(F19:F21)</f>
+        <f t="shared" ref="F22:U22" si="11">SUM(F19:F21)</f>
         <v>2878</v>
       </c>
       <c r="G22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-6207</v>
       </c>
       <c r="H22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6222</v>
       </c>
       <c r="I22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4823</v>
       </c>
       <c r="J22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9185</v>
       </c>
       <c r="K22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8736</v>
       </c>
       <c r="L22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13451</v>
       </c>
       <c r="M22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>22400</v>
       </c>
       <c r="N22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>14324</v>
       </c>
       <c r="O22" s="23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9601</v>
       </c>
       <c r="P22" s="23">
-        <f t="shared" si="10"/>
-        <v>16813.921048554861</v>
+        <f t="shared" si="11"/>
+        <v>14706.455549117749</v>
       </c>
       <c r="Q22" s="23">
-        <f t="shared" si="10"/>
-        <v>17618.790261318056</v>
+        <f t="shared" si="11"/>
+        <v>15015.379729758721</v>
       </c>
       <c r="R22" s="23">
-        <f t="shared" si="10"/>
-        <v>17620.029477876262</v>
+        <f t="shared" si="11"/>
+        <v>15330.437777662466</v>
       </c>
       <c r="S22" s="23">
-        <f t="shared" si="10"/>
-        <v>17405.379728627864</v>
+        <f t="shared" si="11"/>
+        <v>15651.751924010734</v>
       </c>
       <c r="T22" s="23">
-        <f t="shared" si="10"/>
-        <v>17700.949396385029</v>
+        <f t="shared" si="11"/>
+        <v>15979.446840147291</v>
       </c>
       <c r="U22" s="23">
-        <f t="shared" si="10"/>
-        <v>17887.587242680485</v>
+        <f t="shared" si="11"/>
+        <v>16148.869660880368</v>
       </c>
       <c r="W22" s="41">
         <f t="shared" si="1"/>
@@ -12083,139 +12501,143 @@
         <f t="shared" si="2"/>
         <v>-0.10630917563829623</v>
       </c>
-    </row>
-    <row r="23" spans="5:24" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" spans="5:24" x14ac:dyDescent="0.15">
-      <c r="E24" s="49" t="s">
+      <c r="Y22" s="41">
+        <f t="shared" si="3"/>
+        <v>0.10725858014829592</v>
+      </c>
+    </row>
+    <row r="23" spans="5:25" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="5:25" x14ac:dyDescent="0.15">
+      <c r="E24" s="48" t="s">
         <v>72</v>
       </c>
       <c r="F24" s="26" t="str">
-        <f t="shared" ref="F24:N24" si="11">IFERROR(+F11/E11-1,"n/a")</f>
+        <f t="shared" ref="F24:N24" si="12">IFERROR(+F11/E11-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="G24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.36000089613764674</v>
       </c>
       <c r="H24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.26492106276472849</v>
       </c>
       <c r="I24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.20763802407638021</v>
       </c>
       <c r="J24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.4895274760529764E-2</v>
       </c>
       <c r="K24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-3.0640354046242768E-2</v>
       </c>
       <c r="L24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.41662202138314974</v>
       </c>
       <c r="M24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.0391502375980464E-2</v>
       </c>
       <c r="N24" s="26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-0.17329257427263511</v>
       </c>
       <c r="O24" s="26">
-        <f t="shared" ref="O24:U24" si="12">IFERROR(+O11/N11-1,"n/a")</f>
+        <f t="shared" ref="O24:U24" si="13">IFERROR(+O11/N11-1,"n/a")</f>
         <v>3.4208521470910691E-2</v>
       </c>
       <c r="P24" s="26">
-        <f t="shared" si="12"/>
-        <v>0.15955746901437129</v>
+        <f t="shared" si="13"/>
+        <v>2.2089906212943156E-2</v>
       </c>
       <c r="Q24" s="26">
-        <f t="shared" si="12"/>
-        <v>4.5276494766992581E-2</v>
+        <f t="shared" si="13"/>
+        <v>1.9715262479547357E-2</v>
       </c>
       <c r="R24" s="26">
-        <f t="shared" si="12"/>
-        <v>6.6690428056181972E-5</v>
+        <f t="shared" si="13"/>
+        <v>1.9717975295419299E-2</v>
       </c>
       <c r="S24" s="26">
-        <f t="shared" si="12"/>
-        <v>-1.1550950436662766E-2</v>
+        <f t="shared" si="13"/>
+        <v>1.9720663008275352E-2</v>
       </c>
       <c r="T24" s="26">
-        <f t="shared" si="12"/>
-        <v>1.6091365893313059E-2</v>
+        <f t="shared" si="13"/>
+        <v>1.9723325836303651E-2</v>
       </c>
       <c r="U24" s="27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="25" spans="5:24" x14ac:dyDescent="0.15">
-      <c r="E25" s="50" t="s">
+    <row r="25" spans="5:25" x14ac:dyDescent="0.15">
+      <c r="E25" s="49" t="s">
         <v>73</v>
       </c>
       <c r="F25" s="29">
-        <f t="shared" ref="F25:N25" si="13">IFERROR(+F15/F11,"n/a")</f>
+        <f t="shared" ref="F25:N25" si="14">IFERROR(+F15/F11,"n/a")</f>
         <v>0.19423783493144547</v>
       </c>
       <c r="G25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.8155214058179022E-2</v>
       </c>
       <c r="H25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.34741939947419398</v>
       </c>
       <c r="I25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.36656125395297678</v>
       </c>
       <c r="J25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.36382315751445088</v>
       </c>
       <c r="K25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33591111318161704</v>
       </c>
       <c r="L25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.42596642386174915</v>
       </c>
       <c r="M25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.5239177854926419</v>
       </c>
       <c r="N25" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.42611070851218019</v>
       </c>
       <c r="O25" s="29">
-        <f t="shared" ref="O25:U25" si="14">IFERROR(+O15/O11,"n/a")</f>
+        <f t="shared" ref="O25" si="15">IFERROR(+O15/O11,"n/a")</f>
         <v>0.31508498329081175</v>
       </c>
-      <c r="P25" s="54">
-        <f>Input!F29</f>
+      <c r="P25" s="53">
+        <f>Input!F30</f>
         <v>0.42596642386174915</v>
       </c>
-      <c r="Q25" s="54">
-        <f>Input!G29</f>
+      <c r="Q25" s="53">
+        <f>Input!G30</f>
         <v>0.42596642386174915</v>
       </c>
-      <c r="R25" s="54">
-        <f>Input!H29</f>
+      <c r="R25" s="53">
+        <f>Input!H30</f>
         <v>0.42596642386174915</v>
       </c>
-      <c r="S25" s="54">
-        <f>Input!I29</f>
+      <c r="S25" s="53">
+        <f>Input!I30</f>
         <v>0.42596642386174915</v>
       </c>
-      <c r="T25" s="54">
-        <f>Input!J29</f>
+      <c r="T25" s="53">
+        <f>Input!J30</f>
         <v>0.42596642386174915</v>
       </c>
       <c r="U25" s="30">
@@ -12224,8 +12646,8 @@
       </c>
       <c r="W25" s="42"/>
     </row>
-    <row r="26" spans="5:24" x14ac:dyDescent="0.15">
-      <c r="E26" s="50" t="s">
+    <row r="26" spans="5:25" x14ac:dyDescent="0.15">
+      <c r="E26" s="49" t="s">
         <v>139</v>
       </c>
       <c r="F26" s="29">
@@ -12233,59 +12655,59 @@
         <v>0.45506454816285996</v>
       </c>
       <c r="G26" s="29">
-        <f t="shared" ref="G26:U26" si="15">-G20/G19</f>
+        <f t="shared" ref="G26:O26" si="16">-G20/G19</f>
         <v>1.1742043551088777</v>
       </c>
       <c r="H26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.39894046870791056</v>
       </c>
       <c r="I26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.47501864280387768</v>
       </c>
       <c r="J26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.36739982723104525</v>
       </c>
       <c r="K26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.35336787564766842</v>
       </c>
       <c r="L26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.45323360838990284</v>
       </c>
       <c r="M26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.32401846878112078</v>
       </c>
       <c r="N26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.33068548198682307</v>
       </c>
       <c r="O26" s="29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.40173230309072783</v>
       </c>
-      <c r="P26" s="54">
-        <f>Input!F31</f>
+      <c r="P26" s="53">
+        <f>Input!F32</f>
         <v>0.35336787564766842</v>
       </c>
-      <c r="Q26" s="54">
-        <f>Input!G31</f>
+      <c r="Q26" s="53">
+        <f>Input!G32</f>
         <v>0.35336787564766842</v>
       </c>
-      <c r="R26" s="54">
-        <f>Input!H31</f>
+      <c r="R26" s="53">
+        <f>Input!H32</f>
         <v>0.35336787564766842</v>
       </c>
-      <c r="S26" s="54">
-        <f>Input!I31</f>
+      <c r="S26" s="53">
+        <f>Input!I32</f>
         <v>0.35336787564766842</v>
       </c>
-      <c r="T26" s="54">
-        <f>Input!J31</f>
+      <c r="T26" s="53">
+        <f>Input!J32</f>
         <v>0.35336787564766842</v>
       </c>
       <c r="U26" s="30">
@@ -12294,77 +12716,77 @@
       </c>
       <c r="W26" s="42"/>
     </row>
-    <row r="27" spans="5:24" x14ac:dyDescent="0.15">
-      <c r="E27" s="51" t="s">
+    <row r="27" spans="5:25" x14ac:dyDescent="0.15">
+      <c r="E27" s="50" t="s">
         <v>74</v>
       </c>
       <c r="F27" s="32" t="str">
-        <f>IFERROR(+F22/E22-1,"n/a")</f>
+        <f t="shared" ref="F27:O27" si="17">IFERROR(+F22/E22-1,"n/a")</f>
         <v>n/a</v>
       </c>
       <c r="G27" s="32">
-        <f>IFERROR(+G22/F22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>-3.1567060458651843</v>
       </c>
       <c r="H27" s="32">
-        <f>IFERROR(+H22/G22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>-2.00241662638956</v>
       </c>
       <c r="I27" s="32">
-        <f>IFERROR(+I22/H22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>-0.22484731597557051</v>
       </c>
       <c r="J27" s="32">
-        <f>IFERROR(+J22/I22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>0.90441633837860258</v>
       </c>
       <c r="K27" s="32">
-        <f>IFERROR(+K22/J22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>-4.8884050081654862E-2</v>
       </c>
       <c r="L27" s="32">
-        <f>IFERROR(+L22/K22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>0.53972069597069594</v>
       </c>
       <c r="M27" s="32">
-        <f>IFERROR(+M22/L22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>0.66530369489257302</v>
       </c>
       <c r="N27" s="32">
-        <f>IFERROR(+N22/M22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>-0.36053571428571429</v>
       </c>
       <c r="O27" s="32">
-        <f>IFERROR(+O22/N22-1,"n/a")</f>
+        <f t="shared" si="17"/>
         <v>-0.32972633342641722</v>
       </c>
       <c r="P27" s="32">
-        <f t="shared" ref="P27" si="16">IFERROR(+P22/O22-1,"n/a")</f>
-        <v>0.75126768550722445</v>
+        <f t="shared" ref="P27" si="18">IFERROR(+P22/O22-1,"n/a")</f>
+        <v>0.53176289439826574</v>
       </c>
       <c r="Q27" s="32">
-        <f t="shared" ref="Q27" si="17">IFERROR(+Q22/P22-1,"n/a")</f>
-        <v>4.78692156599827E-2</v>
+        <f t="shared" ref="Q27" si="19">IFERROR(+Q22/P22-1,"n/a")</f>
+        <v>2.1006025524586969E-2</v>
       </c>
       <c r="R27" s="32">
-        <f t="shared" ref="R27" si="18">IFERROR(+R22/Q22-1,"n/a")</f>
-        <v>7.0334940130756252E-5</v>
+        <f t="shared" ref="R27" si="20">IFERROR(+R22/Q22-1,"n/a")</f>
+        <v>2.0982356328913765E-2</v>
       </c>
       <c r="S27" s="32">
-        <f t="shared" ref="S27" si="19">IFERROR(+S22/R22-1,"n/a")</f>
-        <v>-1.2182144730115918E-2</v>
+        <f t="shared" ref="S27" si="21">IFERROR(+S22/R22-1,"n/a")</f>
+        <v>2.0959228367010141E-2</v>
       </c>
       <c r="T27" s="32">
-        <f t="shared" ref="T27" si="20">IFERROR(+T22/S22-1,"n/a")</f>
-        <v>1.698151217413657E-2</v>
+        <f t="shared" ref="T27" si="22">IFERROR(+T22/S22-1,"n/a")</f>
+        <v>2.0936628546600833E-2</v>
       </c>
       <c r="U27" s="33">
-        <f t="shared" ref="U27" si="21">IFERROR(+U22/T22-1,"n/a")</f>
-        <v>1.0543945531733545E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="5:24" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="5:24" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" ref="U27" si="23">IFERROR(+U22/T22-1,"n/a")</f>
+        <v>1.0602546034785831E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="5:25" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="5:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E29" s="34" t="s">
         <v>75</v>
       </c>
@@ -12385,7 +12807,7 @@
       <c r="T29" s="18"/>
       <c r="U29" s="18"/>
     </row>
-    <row r="31" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="31" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E31" s="5" t="str">
         <f>Input!$E$8&amp;" Revenues"</f>
         <v>BHP Revenues</v>
@@ -12401,10 +12823,11 @@
         <v>111</v>
       </c>
       <c r="X31" s="39"/>
-    </row>
-    <row r="32" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y31" s="39"/>
+    </row>
+    <row r="32" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E32" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F32" s="37" t="s">
@@ -12461,9 +12884,12 @@
       <c r="X32" s="39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="33" spans="5:26" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" spans="5:26" x14ac:dyDescent="0.15">
+      <c r="Y32" s="39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="5:27" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E34" s="13" t="s">
         <v>106</v>
       </c>
@@ -12497,12 +12923,12 @@
       <c r="O34" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
-      <c r="R34" s="52"/>
-      <c r="S34" s="52"/>
-      <c r="T34" s="52"/>
-      <c r="U34" s="52"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="51"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="51"/>
+      <c r="T34" s="51"/>
+      <c r="U34" s="51"/>
       <c r="W34" s="29" t="str">
         <f>IFERROR((O34/F34)^(1/9)-1,"n/a")</f>
         <v>n/a</v>
@@ -12511,11 +12937,15 @@
         <f>IFERROR((O34/L34)^(1/3)-1,"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="Z34" s="35" t="s">
+      <c r="Y34" s="29" t="str">
+        <f t="shared" ref="Y34:Y39" si="24">IFERROR((T34/O34)^(1/5)-1,"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="AA34" s="35" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="5:26" x14ac:dyDescent="0.15">
+    <row r="35" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E35" s="13" t="s">
         <v>88</v>
       </c>
@@ -12551,41 +12981,45 @@
       </c>
       <c r="P35" s="18">
         <f>P42*P47/10^3</f>
-        <v>20308.240811041433</v>
+        <v>18937.319999999996</v>
       </c>
       <c r="Q35" s="18">
-        <f t="shared" ref="Q35:U35" si="22">Q42*Q47/10^3</f>
-        <v>20815.946831317469</v>
+        <f t="shared" ref="Q35:U35" si="25">Q42*Q47/10^3</f>
+        <v>19316.0664</v>
       </c>
       <c r="R35" s="18">
-        <f t="shared" si="22"/>
-        <v>21323.652851593506</v>
+        <f t="shared" si="25"/>
+        <v>19702.387728000002</v>
       </c>
       <c r="S35" s="18">
-        <f t="shared" si="22"/>
-        <v>21831.358871869543</v>
+        <f t="shared" si="25"/>
+        <v>20096.435482560002</v>
       </c>
       <c r="T35" s="18">
-        <f t="shared" si="22"/>
-        <v>22339.064892145576</v>
+        <f t="shared" si="25"/>
+        <v>20498.364192211204</v>
       </c>
       <c r="U35" s="18">
-        <f t="shared" si="22"/>
-        <v>22562.455541067029</v>
+        <f t="shared" si="25"/>
+        <v>20703.347834133314</v>
       </c>
       <c r="W35" s="29">
-        <f t="shared" ref="W35:W39" si="23">IFERROR((O35/F35)^(1/9)-1,"n/a")</f>
+        <f t="shared" ref="W35:W39" si="26">IFERROR((O35/F35)^(1/9)-1,"n/a")</f>
         <v>5.5142240492537464E-2</v>
       </c>
       <c r="X35" s="29">
-        <f t="shared" ref="X35:X39" si="24">IFERROR((O35/L35)^(1/3)-1,"n/a")</f>
+        <f t="shared" ref="X35:X39" si="27">IFERROR((O35/L35)^(1/3)-1,"n/a")</f>
         <v>5.6898686735249449E-2</v>
       </c>
-      <c r="Z35" s="35" t="s">
+      <c r="Y35" s="29">
+        <f t="shared" si="24"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="AA35" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="5:26" x14ac:dyDescent="0.15">
+    <row r="36" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E36" s="13" t="s">
         <v>93</v>
       </c>
@@ -12621,41 +13055,45 @@
       </c>
       <c r="P36" s="18">
         <f>P43*P48/10^3</f>
-        <v>32381.920165978419</v>
+        <v>28511.039999999997</v>
       </c>
       <c r="Q36" s="18">
-        <f t="shared" ref="Q36:U36" si="25">Q43*Q48/10^3</f>
-        <v>33418.404067522169</v>
+        <f t="shared" ref="Q36:U36" si="28">Q43*Q48/10^3</f>
+        <v>29081.260799999996</v>
       </c>
       <c r="R36" s="18">
-        <f t="shared" si="25"/>
-        <v>32140.839476307272</v>
+        <f t="shared" si="28"/>
+        <v>29662.886016</v>
       </c>
       <c r="S36" s="18">
-        <f t="shared" si="25"/>
-        <v>32493.242618220364</v>
+        <f t="shared" si="28"/>
+        <v>30256.143736319995</v>
       </c>
       <c r="T36" s="18">
-        <f t="shared" si="25"/>
-        <v>32935.684376127974</v>
+        <f t="shared" si="28"/>
+        <v>30861.266611046398</v>
       </c>
       <c r="U36" s="18">
-        <f t="shared" si="25"/>
-        <v>33265.041219889259</v>
+        <f t="shared" si="28"/>
+        <v>31169.879277156859</v>
       </c>
       <c r="W36" s="29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>7.3586271885691446E-2</v>
       </c>
       <c r="X36" s="29">
+        <f t="shared" si="27"/>
+        <v>-6.7527131592702072E-2</v>
+      </c>
+      <c r="Y36" s="29">
         <f t="shared" si="24"/>
-        <v>-6.7527131592702072E-2</v>
-      </c>
-      <c r="Z36" s="35" t="s">
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="AA36" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="5:26" x14ac:dyDescent="0.15">
+    <row r="37" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E37" s="13" t="s">
         <v>94</v>
       </c>
@@ -12691,41 +13129,45 @@
       </c>
       <c r="P37" s="18">
         <f>P44*P49/10^3</f>
-        <v>10112.738633382023</v>
+        <v>7819.32</v>
       </c>
       <c r="Q37" s="18">
-        <f t="shared" ref="Q37:U37" si="26">Q44*Q49/10^3</f>
-        <v>11473.275042916373</v>
+        <f t="shared" ref="Q37:U37" si="29">Q44*Q49/10^3</f>
+        <v>7975.7064</v>
       </c>
       <c r="R37" s="18">
+        <f t="shared" si="29"/>
+        <v>8135.2205279999998</v>
+      </c>
+      <c r="S37" s="18">
+        <f t="shared" si="29"/>
+        <v>8297.9249385600015</v>
+      </c>
+      <c r="T37" s="18">
+        <f t="shared" si="29"/>
+        <v>8463.883437331202</v>
+      </c>
+      <c r="U37" s="18">
+        <f t="shared" si="29"/>
+        <v>8548.5222717045144</v>
+      </c>
+      <c r="W37" s="29">
         <f t="shared" si="26"/>
-        <v>12230.10152404544</v>
-      </c>
-      <c r="S37" s="18">
-        <f t="shared" si="26"/>
-        <v>10572.998420144733</v>
-      </c>
-      <c r="T37" s="18">
-        <f t="shared" si="26"/>
-        <v>10678.035131213901</v>
-      </c>
-      <c r="U37" s="18">
-        <f t="shared" si="26"/>
-        <v>10784.815482526039</v>
-      </c>
-      <c r="W37" s="29">
-        <f t="shared" si="23"/>
         <v>2.9812214481835575E-2</v>
       </c>
       <c r="X37" s="29">
+        <f t="shared" si="27"/>
+        <v>0.14149706778136784</v>
+      </c>
+      <c r="Y37" s="29">
         <f t="shared" si="24"/>
-        <v>0.14149706778136784</v>
-      </c>
-      <c r="Z37" s="35" t="s">
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="AA37" s="35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="5:26" x14ac:dyDescent="0.15">
+    <row r="38" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E38" s="13" t="s">
         <v>95</v>
       </c>
@@ -12760,64 +13202,68 @@
         <v>1474</v>
       </c>
       <c r="P38" s="18">
-        <f>AVERAGE(L38:O38)</f>
-        <v>1735.75</v>
+        <f>AVERAGE(K38:O38)</f>
+        <v>1619.8</v>
       </c>
       <c r="Q38" s="18">
         <f>P38*(1+$B$3)</f>
-        <v>1753.1075000000001</v>
+        <v>1635.998</v>
       </c>
       <c r="R38" s="18">
         <f>Q38*(1+$B$3)</f>
-        <v>1770.6385750000002</v>
+        <v>1652.35798</v>
       </c>
       <c r="S38" s="18">
         <f>R38*(1+$B$3)</f>
-        <v>1788.3449607500002</v>
+        <v>1668.8815598000001</v>
       </c>
       <c r="T38" s="18">
         <f>S38*(1+$B$3)</f>
-        <v>1806.2284103575003</v>
+        <v>1685.5703753980001</v>
       </c>
       <c r="U38" s="18">
         <f>T38*(1+$B$3)</f>
-        <v>1824.2906944610752</v>
+        <v>1702.42607915198</v>
       </c>
       <c r="W38" s="29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>3.326227060457887E-2</v>
       </c>
       <c r="X38" s="29">
+        <f t="shared" si="27"/>
+        <v>-9.3214479088485902E-3</v>
+      </c>
+      <c r="Y38" s="29">
         <f t="shared" si="24"/>
-        <v>-9.3214479088485902E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="5:26" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+        <v>2.7187867752968886E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="5:27" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="E39" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F39" s="23">
-        <f t="shared" ref="F39:K39" si="27">SUM(F34:F38)</f>
+        <f t="shared" ref="F39:K39" si="30">SUM(F34:F38)</f>
         <v>44636</v>
       </c>
       <c r="G39" s="23">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>28567</v>
       </c>
       <c r="H39" s="23">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>36135</v>
       </c>
       <c r="I39" s="23">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>43638</v>
       </c>
       <c r="J39" s="23">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>44288</v>
       </c>
       <c r="K39" s="23">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>42931</v>
       </c>
       <c r="L39" s="23">
@@ -12825,122 +13271,126 @@
         <v>60817</v>
       </c>
       <c r="M39" s="23">
-        <f t="shared" ref="M39:U39" si="28">SUM(M34:M38)</f>
+        <f t="shared" ref="M39:U39" si="31">SUM(M34:M38)</f>
         <v>65098</v>
       </c>
       <c r="N39" s="23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>53817</v>
       </c>
       <c r="O39" s="23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>55658</v>
       </c>
       <c r="P39" s="23">
-        <f t="shared" si="28"/>
-        <v>64538.649610401881</v>
+        <f>SUM(P34:P38)</f>
+        <v>56887.479999999996</v>
       </c>
       <c r="Q39" s="23">
-        <f t="shared" si="28"/>
-        <v>67460.733441756005</v>
+        <f t="shared" si="31"/>
+        <v>58009.031600000002</v>
       </c>
       <c r="R39" s="23">
-        <f t="shared" si="28"/>
-        <v>67465.232426946226</v>
+        <f t="shared" si="31"/>
+        <v>59152.852252000004</v>
       </c>
       <c r="S39" s="23">
-        <f t="shared" si="28"/>
-        <v>66685.944870984633</v>
+        <f t="shared" si="31"/>
+        <v>60319.385717239995</v>
       </c>
       <c r="T39" s="23">
-        <f t="shared" si="28"/>
-        <v>67759.01280984495</v>
+        <f t="shared" si="31"/>
+        <v>61509.084615986802</v>
       </c>
       <c r="U39" s="23">
-        <f t="shared" si="28"/>
-        <v>68436.602937943404</v>
+        <f t="shared" si="31"/>
+        <v>62124.175462146668</v>
       </c>
       <c r="W39" s="41">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>2.4823669769025392E-2</v>
       </c>
       <c r="X39" s="41">
+        <f t="shared" si="27"/>
+        <v>-2.9115574512328934E-2</v>
+      </c>
+      <c r="Y39" s="41">
         <f t="shared" si="24"/>
-        <v>-2.9115574512328934E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="5:26" x14ac:dyDescent="0.15">
+        <v>2.0192986291499571E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E41" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="5:26" x14ac:dyDescent="0.15">
-      <c r="E42" s="48" t="s">
+    <row r="42" spans="5:27" x14ac:dyDescent="0.15">
+      <c r="E42" t="s">
         <v>128</v>
       </c>
-      <c r="F42" s="55">
+      <c r="F42" s="54">
         <f>[1]Prices!AC11</f>
         <v>5510.4571127155004</v>
       </c>
-      <c r="G42" s="55">
+      <c r="G42" s="54">
         <f>[1]Prices!AD11</f>
         <v>4867.897429653679</v>
       </c>
-      <c r="H42" s="55">
+      <c r="H42" s="54">
         <f>[1]Prices!AE11</f>
         <v>6169.9399418513613</v>
       </c>
-      <c r="I42" s="55">
+      <c r="I42" s="54">
         <f>[1]Prices!AF11</f>
         <v>6529.7983709685941</v>
       </c>
-      <c r="J42" s="55">
+      <c r="J42" s="54">
         <f>[1]Prices!AG11</f>
         <v>6010.145429645836</v>
       </c>
-      <c r="K42" s="55">
+      <c r="K42" s="54">
         <f>[1]Prices!AH11</f>
         <v>6174.5579173221258</v>
       </c>
-      <c r="L42" s="55">
+      <c r="L42" s="54">
         <f>[1]Prices!AI11</f>
         <v>9317.4091658824254</v>
       </c>
-      <c r="M42" s="55">
+      <c r="M42" s="54">
         <f>[1]Prices!AJ11</f>
         <v>8828.9168140645579</v>
       </c>
-      <c r="N42" s="55">
+      <c r="N42" s="54">
         <f>[1]Prices!AK11</f>
         <v>8490.7617314997788</v>
       </c>
-      <c r="O42" s="55">
+      <c r="O42" s="54">
         <f>[1]Prices!AL11</f>
         <v>9142.1015600257251</v>
       </c>
-      <c r="P42" s="55">
-        <f>Input!F20</f>
-        <v>10000</v>
-      </c>
-      <c r="Q42" s="55">
-        <f>Input!G20</f>
-        <v>10250</v>
-      </c>
-      <c r="R42" s="55">
-        <f>Input!H20</f>
-        <v>10500</v>
-      </c>
-      <c r="S42" s="55">
-        <f>Input!I20</f>
-        <v>10750</v>
-      </c>
-      <c r="T42" s="55">
-        <f>Input!J20</f>
-        <v>11000</v>
+      <c r="P42" s="54">
+        <f>Input!F21</f>
+        <v>9324.9435912262397</v>
+      </c>
+      <c r="Q42" s="54">
+        <f>Input!G21</f>
+        <v>9511.4424630507656</v>
+      </c>
+      <c r="R42" s="54">
+        <f>Input!H21</f>
+        <v>9701.6713123117806</v>
+      </c>
+      <c r="S42" s="54">
+        <f>Input!I21</f>
+        <v>9895.7047385580172</v>
+      </c>
+      <c r="T42" s="54">
+        <f>Input!J21</f>
+        <v>10093.618833329178</v>
       </c>
       <c r="U42" s="18">
         <f>T42</f>
-        <v>11000</v>
+        <v>10093.618833329178</v>
       </c>
       <c r="W42" s="29">
         <f>IFERROR((O42/F42)^(1/9)-1,"n/a")</f>
@@ -12950,77 +13400,81 @@
         <f>IFERROR((O42/L42)^(1/3)-1,"n/a")</f>
         <v>-6.3114368604682003E-3</v>
       </c>
-      <c r="Z42" s="35" t="s">
+      <c r="Y42" s="29">
+        <f t="shared" ref="Y42:Y44" si="32">IFERROR((T42/O42)^(1/5)-1,"n/a")</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="AA42" s="35" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="5:26" x14ac:dyDescent="0.15">
+    <row r="43" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E43" t="s">
         <v>129</v>
       </c>
-      <c r="F43" s="55">
+      <c r="F43" s="54">
         <f>[1]Prices!AC12</f>
         <v>56.137484315201696</v>
       </c>
-      <c r="G43" s="55">
+      <c r="G43" s="54">
         <f>[1]Prices!AD12</f>
         <v>58.56519072714724</v>
       </c>
-      <c r="H43" s="55">
+      <c r="H43" s="54">
         <f>[1]Prices!AE12</f>
         <v>71.134474402409182</v>
       </c>
-      <c r="I43" s="55">
+      <c r="I43" s="54">
         <f>[1]Prices!AF12</f>
         <v>70.13840422862161</v>
       </c>
-      <c r="J43" s="55">
+      <c r="J43" s="54">
         <f>[1]Prices!AG12</f>
         <v>93.624179214505304</v>
       </c>
-      <c r="K43" s="55">
+      <c r="K43" s="54">
         <f>[1]Prices!AH12</f>
         <v>108.07149327122153</v>
       </c>
-      <c r="L43" s="55">
+      <c r="L43" s="54">
         <f>[1]Prices!AI12</f>
         <v>158.16166811235101</v>
       </c>
-      <c r="M43" s="55">
+      <c r="M43" s="54">
         <f>[1]Prices!AJ12</f>
         <v>120.7038647342995</v>
       </c>
-      <c r="N43" s="55">
+      <c r="N43" s="54">
         <f>[1]Prices!AK12</f>
         <v>120.31531698977351</v>
       </c>
-      <c r="O43" s="55">
+      <c r="O43" s="54">
         <f>[1]Prices!AL12</f>
         <v>111.06139108476066</v>
       </c>
-      <c r="P43" s="55">
-        <f>Input!F21</f>
-        <v>128.66274683848124</v>
-      </c>
-      <c r="Q43" s="55">
-        <f>Input!G21</f>
-        <v>132.78099755193318</v>
-      </c>
-      <c r="R43" s="55">
-        <f>Input!H21</f>
-        <v>127.70486343984962</v>
-      </c>
-      <c r="S43" s="55">
-        <f>Input!I21</f>
-        <v>129.10506318095966</v>
-      </c>
-      <c r="T43" s="55">
-        <f>Input!J21</f>
-        <v>130.86301241919688</v>
+      <c r="P43" s="54">
+        <f>Input!F22</f>
+        <v>113.28261890645587</v>
+      </c>
+      <c r="Q43" s="54">
+        <f>Input!G22</f>
+        <v>115.54827128458498</v>
+      </c>
+      <c r="R43" s="54">
+        <f>Input!H22</f>
+        <v>117.85923671027669</v>
+      </c>
+      <c r="S43" s="54">
+        <f>Input!I22</f>
+        <v>120.21642144448222</v>
+      </c>
+      <c r="T43" s="54">
+        <f>Input!J22</f>
+        <v>122.62074987337186</v>
       </c>
       <c r="U43" s="18">
         <f>T43</f>
-        <v>130.86301241919688</v>
+        <v>122.62074987337186</v>
       </c>
       <c r="W43" s="29">
         <f>IFERROR((O43/F43)^(1/9)-1,"n/a")</f>
@@ -13030,74 +13484,78 @@
         <f>IFERROR((O43/L43)^(1/3)-1,"n/a")</f>
         <v>-0.11116607165505865</v>
       </c>
-    </row>
-    <row r="44" spans="5:26" x14ac:dyDescent="0.15">
+      <c r="Y43" s="29">
+        <f t="shared" si="32"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E44" t="s">
         <v>130</v>
       </c>
-      <c r="F44" s="55">
+      <c r="F44" s="54">
         <f>[1]Prices!AC10</f>
         <v>62.692552690750638</v>
       </c>
-      <c r="G44" s="55">
+      <c r="G44" s="54">
         <f>[1]Prices!AD10</f>
         <v>70.08180639301159</v>
       </c>
-      <c r="H44" s="55">
+      <c r="H44" s="54">
         <f>[1]Prices!AE10</f>
         <v>94.138079349276438</v>
       </c>
-      <c r="I44" s="55">
+      <c r="I44" s="54">
         <f>[1]Prices!AF10</f>
         <v>113.23078537013389</v>
       </c>
-      <c r="J44" s="55">
+      <c r="J44" s="54">
         <f>[1]Prices!AG10</f>
         <v>82.193236275241134</v>
       </c>
-      <c r="K44" s="55">
+      <c r="K44" s="54">
         <f>[1]Prices!AH10</f>
         <v>61.983198111650417</v>
       </c>
-      <c r="L44" s="55">
+      <c r="L44" s="54">
         <f>[1]Prices!AI10</f>
         <v>143.98474438540202</v>
       </c>
-      <c r="M44" s="55">
+      <c r="M44" s="54">
         <f>[1]Prices!AJ10</f>
         <v>384.16973325553721</v>
       </c>
-      <c r="N44" s="55">
+      <c r="N44" s="54">
         <f>[1]Prices!AK10</f>
         <v>188.15258386900859</v>
       </c>
-      <c r="O44" s="55">
+      <c r="O44" s="54">
         <f>[1]Prices!AL10</f>
         <v>143.55138180272291</v>
       </c>
-      <c r="P44" s="55">
-        <f>Input!F22</f>
-        <v>189.36832828486422</v>
-      </c>
-      <c r="Q44" s="55">
-        <f>Input!G22</f>
-        <v>214.84535431950698</v>
-      </c>
-      <c r="R44" s="55">
-        <f>Input!H22</f>
-        <v>229.01747630632798</v>
-      </c>
-      <c r="S44" s="55">
-        <f>Input!I22</f>
-        <v>197.98702491648615</v>
-      </c>
-      <c r="T44" s="55">
-        <f>Input!J22</f>
-        <v>199.95391312598164</v>
+      <c r="P44" s="54">
+        <f>Input!F23</f>
+        <v>146.42240943877738</v>
+      </c>
+      <c r="Q44" s="54">
+        <f>Input!G23</f>
+        <v>149.35085762755293</v>
+      </c>
+      <c r="R44" s="54">
+        <f>Input!H23</f>
+        <v>152.33787478010399</v>
+      </c>
+      <c r="S44" s="54">
+        <f>Input!I23</f>
+        <v>155.38463227570608</v>
+      </c>
+      <c r="T44" s="54">
+        <f>Input!J23</f>
+        <v>158.49232492122022</v>
       </c>
       <c r="U44" s="18">
         <f>T44</f>
-        <v>199.95391312598164</v>
+        <v>158.49232492122022</v>
       </c>
       <c r="W44" s="29">
         <f>IFERROR((O44/F44)^(1/9)-1,"n/a")</f>
@@ -13107,8 +13565,12 @@
         <f>IFERROR((O44/L44)^(1/3)-1,"n/a")</f>
         <v>-1.0042686316182881E-3</v>
       </c>
-    </row>
-    <row r="45" spans="5:26" x14ac:dyDescent="0.15">
+      <c r="Y44" s="29">
+        <f t="shared" si="32"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="5:27" x14ac:dyDescent="0.15">
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
@@ -13126,7 +13588,7 @@
       <c r="T45" s="18"/>
       <c r="U45" s="18"/>
     </row>
-    <row r="46" spans="5:26" x14ac:dyDescent="0.15">
+    <row r="46" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E46" s="5" t="str">
         <f>Input!$E$8&amp;" Indicative volumes (thousand tons)"</f>
         <v>BHP Indicative volumes (thousand tons)</v>
@@ -13148,7 +13610,7 @@
       <c r="T46" s="18"/>
       <c r="U46" s="18"/>
     </row>
-    <row r="47" spans="5:26" x14ac:dyDescent="0.15">
+    <row r="47" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E47" t="s">
         <v>88</v>
       </c>
@@ -13157,39 +13619,39 @@
         <v>2078.4119657826486</v>
       </c>
       <c r="G47" s="18">
-        <f t="shared" ref="G47:O47" si="29">G35/G42*10^3</f>
+        <f t="shared" ref="G47:O47" si="33">G35/G42*10^3</f>
         <v>1694.5714488045132</v>
       </c>
       <c r="H47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1350.9045596153708</v>
       </c>
       <c r="I47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>2034.8254639950055</v>
       </c>
       <c r="J47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1803.2841512520038</v>
       </c>
       <c r="K47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1727.4111187907993</v>
       </c>
       <c r="L47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1687.8082436890206</v>
       </c>
       <c r="M47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1908.3881244819709</v>
       </c>
       <c r="N47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1887.5809387680281</v>
       </c>
       <c r="O47" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>2030.8240811041433</v>
       </c>
       <c r="P47" s="18">
@@ -13197,23 +13659,23 @@
         <v>2030.8240811041433</v>
       </c>
       <c r="Q47" s="18">
-        <f t="shared" ref="Q47:U47" si="30">P47*(1+Q51)</f>
+        <f t="shared" ref="Q47:U47" si="34">P47*(1+Q51)</f>
         <v>2030.8240811041433</v>
       </c>
       <c r="R47" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>2030.8240811041433</v>
       </c>
       <c r="S47" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>2030.8240811041433</v>
       </c>
       <c r="T47" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>2030.8240811041433</v>
       </c>
       <c r="U47" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>2051.1323219151845</v>
       </c>
       <c r="W47" s="29">
@@ -13224,8 +13686,12 @@
         <f>IFERROR((O47/L47)^(1/3)-1,"n/a")</f>
         <v>6.3611604219340867E-2</v>
       </c>
-    </row>
-    <row r="48" spans="5:26" x14ac:dyDescent="0.15">
+      <c r="Y47" s="29">
+        <f t="shared" ref="Y47:Y49" si="35">IFERROR((T47/O47)^(1/5)-1,"n/a")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="5:27" x14ac:dyDescent="0.15">
       <c r="E48" t="s">
         <v>93</v>
       </c>
@@ -13234,63 +13700,63 @@
         <v>262801.23129787232</v>
       </c>
       <c r="G48" s="18">
-        <f t="shared" ref="G48:O48" si="31">G36/G43*10^3</f>
+        <f t="shared" ref="G48:O48" si="36">G36/G43*10^3</f>
         <v>179936.23634039031</v>
       </c>
       <c r="H48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>205582.45664783759</v>
       </c>
       <c r="I48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>211153.93432285183</v>
       </c>
       <c r="J48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>184300.68113565541</v>
       </c>
       <c r="K48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>192437.42610094993</v>
       </c>
       <c r="L48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>217973.16891922572</v>
       </c>
       <c r="M48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>254896.56083279639</v>
       </c>
       <c r="N48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>206224.78185474055</v>
       </c>
       <c r="O48" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>251680.62210446637</v>
       </c>
       <c r="P48" s="18">
-        <f t="shared" ref="P48:U48" si="32">O48*(1+P52)</f>
+        <f t="shared" ref="P48:U48" si="37">O48*(1+P52)</f>
         <v>251680.62210446637</v>
       </c>
       <c r="Q48" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>251680.62210446637</v>
       </c>
       <c r="R48" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>251680.62210446637</v>
       </c>
       <c r="S48" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>251680.62210446637</v>
       </c>
       <c r="T48" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>251680.62210446637</v>
       </c>
       <c r="U48" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>254197.42832551102</v>
       </c>
       <c r="W48" s="29">
@@ -13301,8 +13767,12 @@
         <f>IFERROR((O48/L48)^(1/3)-1,"n/a")</f>
         <v>4.9096843258014111E-2</v>
       </c>
-    </row>
-    <row r="49" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y48" s="29">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:25" x14ac:dyDescent="0.15">
       <c r="E49" t="s">
         <v>94</v>
       </c>
@@ -13311,63 +13781,63 @@
         <v>93870.798801725061</v>
       </c>
       <c r="G49" s="18">
-        <f t="shared" ref="G49:O49" si="33">G37/G44*10^3</f>
+        <f t="shared" ref="G49:O49" si="38">G37/G44*10^3</f>
         <v>64467.516357434033</v>
       </c>
       <c r="H49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>80498.774272668932</v>
       </c>
       <c r="I49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>78503.38554963861</v>
       </c>
       <c r="J49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>110970.20160462397</v>
       </c>
       <c r="K49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>100704.71014993897</v>
       </c>
       <c r="L49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>35795.458900870479</v>
       </c>
       <c r="M49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>40474.297306647291</v>
       </c>
       <c r="N49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>58239.965535785224</v>
       </c>
       <c r="O49" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>53402.481423237608</v>
       </c>
       <c r="P49" s="18">
-        <f t="shared" ref="P49:U49" si="34">O49*(1+P53)</f>
+        <f t="shared" ref="P49:U49" si="39">O49*(1+P53)</f>
         <v>53402.481423237608</v>
       </c>
       <c r="Q49" s="18">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>53402.481423237608</v>
       </c>
       <c r="R49" s="18">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>53402.481423237608</v>
       </c>
       <c r="S49" s="18">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>53402.481423237608</v>
       </c>
       <c r="T49" s="18">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>53402.481423237608</v>
       </c>
       <c r="U49" s="18">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>53936.506237469985</v>
       </c>
       <c r="W49" s="29">
@@ -13378,8 +13848,12 @@
         <f>IFERROR((O49/L49)^(1/3)-1,"n/a")</f>
         <v>0.14264458990009277</v>
       </c>
-    </row>
-    <row r="50" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y49" s="29">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
       <c r="H50" s="18"/>
@@ -13397,8 +13871,8 @@
       <c r="T50" s="18"/>
       <c r="U50" s="18"/>
     </row>
-    <row r="51" spans="5:24" x14ac:dyDescent="0.15">
-      <c r="E51" s="49" t="s">
+    <row r="51" spans="5:25" x14ac:dyDescent="0.15">
+      <c r="E51" s="48" t="s">
         <v>131</v>
       </c>
       <c r="F51" s="26" t="s">
@@ -13409,50 +13883,50 @@
         <v>-0.18467970897848254</v>
       </c>
       <c r="H51" s="26">
-        <f t="shared" ref="H51:O51" si="35">(H47-G47)/G47</f>
+        <f t="shared" ref="H51:O51" si="40">(H47-G47)/G47</f>
         <v>-0.20280460256284424</v>
       </c>
       <c r="I51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>0.50626885482891593</v>
       </c>
       <c r="J51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>-0.11378927423505551</v>
       </c>
       <c r="K51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>-4.2074917815102267E-2</v>
       </c>
       <c r="L51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>-2.2926143447253567E-2</v>
       </c>
       <c r="M51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>0.13069013119098863</v>
       </c>
       <c r="N51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>-1.0903015716255755E-2</v>
       </c>
       <c r="O51" s="26">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>7.588715238330708E-2</v>
       </c>
-      <c r="P51" s="60">
+      <c r="P51" s="59">
         <v>0</v>
       </c>
-      <c r="Q51" s="60">
+      <c r="Q51" s="59">
         <v>0</v>
       </c>
-      <c r="R51" s="60">
+      <c r="R51" s="59">
         <v>0</v>
       </c>
-      <c r="S51" s="60">
+      <c r="S51" s="59">
         <v>0</v>
       </c>
-      <c r="T51" s="60">
+      <c r="T51" s="59">
         <v>0</v>
       </c>
       <c r="U51" s="27">
@@ -13461,138 +13935,141 @@
       </c>
       <c r="W51" s="29"/>
       <c r="X51" s="29"/>
-    </row>
-    <row r="52" spans="5:24" x14ac:dyDescent="0.15">
-      <c r="E52" s="50" t="s">
+      <c r="Y51" s="29"/>
+    </row>
+    <row r="52" spans="5:25" x14ac:dyDescent="0.15">
+      <c r="E52" s="49" t="s">
         <v>132</v>
       </c>
       <c r="F52" s="29" t="s">
         <v>107</v>
       </c>
       <c r="G52" s="29">
-        <f t="shared" ref="G52:O53" si="36">(G48-F48)/F48</f>
+        <f t="shared" ref="G52:O53" si="41">(G48-F48)/F48</f>
         <v>-0.31531433299701173</v>
       </c>
       <c r="H52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.14252949171911999</v>
       </c>
       <c r="I52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>2.7100939281789815E-2</v>
       </c>
       <c r="J52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.12717382355821094</v>
       </c>
       <c r="K52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>4.4149294051200119E-2</v>
       </c>
       <c r="L52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.13269634361498941</v>
       </c>
       <c r="M52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.16939420616146275</v>
       </c>
       <c r="N52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.19094717802011812</v>
       </c>
       <c r="O52" s="29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.22041890330010749</v>
       </c>
-      <c r="P52" s="54">
+      <c r="P52" s="53">
         <v>0</v>
       </c>
-      <c r="Q52" s="54">
+      <c r="Q52" s="53">
         <v>0</v>
       </c>
-      <c r="R52" s="54">
+      <c r="R52" s="53">
         <v>0</v>
       </c>
-      <c r="S52" s="54">
+      <c r="S52" s="53">
         <v>0</v>
       </c>
-      <c r="T52" s="54">
+      <c r="T52" s="53">
         <v>0</v>
       </c>
       <c r="U52" s="30">
-        <f t="shared" ref="U52:U53" si="37">$B$3</f>
+        <f t="shared" ref="U52:U53" si="42">$B$3</f>
         <v>0.01</v>
       </c>
       <c r="W52" s="29"/>
       <c r="X52" s="29"/>
-    </row>
-    <row r="53" spans="5:24" x14ac:dyDescent="0.15">
-      <c r="E53" s="51" t="s">
+      <c r="Y52" s="29"/>
+    </row>
+    <row r="53" spans="5:25" x14ac:dyDescent="0.15">
+      <c r="E53" s="50" t="s">
         <v>133</v>
       </c>
       <c r="F53" s="32" t="s">
         <v>107</v>
       </c>
       <c r="G53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.31323140763292073</v>
       </c>
       <c r="H53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.24867187106063013</v>
       </c>
       <c r="I53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-2.4787814983013971E-2</v>
       </c>
       <c r="J53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.41357217688982617</v>
       </c>
       <c r="K53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-9.2506738802367428E-2</v>
       </c>
       <c r="L53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-0.64455030109738942</v>
       </c>
       <c r="M53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.13071039035242071</v>
       </c>
       <c r="N53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>0.43893703933978345</v>
       </c>
       <c r="O53" s="32">
-        <f t="shared" si="36"/>
+        <f t="shared" si="41"/>
         <v>-8.3061246139908007E-2</v>
       </c>
-      <c r="P53" s="61">
+      <c r="P53" s="60">
         <v>0</v>
       </c>
-      <c r="Q53" s="61">
+      <c r="Q53" s="60">
         <v>0</v>
       </c>
-      <c r="R53" s="61">
+      <c r="R53" s="60">
         <v>0</v>
       </c>
-      <c r="S53" s="61">
+      <c r="S53" s="60">
         <v>0</v>
       </c>
-      <c r="T53" s="61">
+      <c r="T53" s="60">
         <v>0</v>
       </c>
       <c r="U53" s="33">
-        <f t="shared" si="37"/>
+        <f t="shared" si="42"/>
         <v>0.01</v>
       </c>
       <c r="W53" s="29"/>
       <c r="X53" s="29"/>
-    </row>
-    <row r="54" spans="5:24" x14ac:dyDescent="0.15">
+      <c r="Y53" s="29"/>
+    </row>
+    <row r="54" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
       <c r="H54" s="18"/>
@@ -13610,7 +14087,7 @@
       <c r="T54" s="18"/>
       <c r="U54" s="18"/>
     </row>
-    <row r="55" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="55" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
       <c r="H55" s="18"/>
@@ -13628,7 +14105,7 @@
       <c r="T55" s="18"/>
       <c r="U55" s="3"/>
     </row>
-    <row r="56" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="56" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F56" s="18"/>
       <c r="G56" s="18"/>
       <c r="H56" s="18"/>
@@ -13646,7 +14123,7 @@
       <c r="T56" s="18"/>
       <c r="U56" s="18"/>
     </row>
-    <row r="57" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="57" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
       <c r="H57" s="18"/>
@@ -13664,7 +14141,7 @@
       <c r="T57" s="18"/>
       <c r="U57" s="18"/>
     </row>
-    <row r="58" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="58" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
       <c r="H58" s="18"/>
@@ -13682,7 +14159,7 @@
       <c r="T58" s="18"/>
       <c r="U58" s="18"/>
     </row>
-    <row r="59" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="59" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
       <c r="H59" s="18"/>
@@ -13700,7 +14177,7 @@
       <c r="T59" s="18"/>
       <c r="U59" s="18"/>
     </row>
-    <row r="60" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="60" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
       <c r="H60" s="18"/>
@@ -13718,7 +14195,7 @@
       <c r="T60" s="18"/>
       <c r="U60" s="18"/>
     </row>
-    <row r="61" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="61" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
       <c r="H61" s="18"/>
@@ -13736,7 +14213,7 @@
       <c r="T61" s="18"/>
       <c r="U61" s="18"/>
     </row>
-    <row r="62" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="62" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
       <c r="H62" s="18"/>
@@ -13754,7 +14231,7 @@
       <c r="T62" s="18"/>
       <c r="U62" s="18"/>
     </row>
-    <row r="63" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="63" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F63" s="18"/>
       <c r="G63" s="18"/>
       <c r="H63" s="18"/>
@@ -13772,7 +14249,7 @@
       <c r="T63" s="18"/>
       <c r="U63" s="18"/>
     </row>
-    <row r="64" spans="5:24" x14ac:dyDescent="0.15">
+    <row r="64" spans="5:25" x14ac:dyDescent="0.15">
       <c r="F64" s="18"/>
       <c r="G64" s="18"/>
       <c r="H64" s="18"/>
@@ -26102,8 +26579,8 @@
   </sheetPr>
   <dimension ref="A1:T810"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
@@ -26159,7 +26636,7 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.15">
       <c r="E9" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F9" s="37" t="s">
@@ -26758,7 +27235,7 @@
     </row>
     <row r="23" spans="3:18" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="24" spans="3:18" x14ac:dyDescent="0.15">
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="48" t="s">
         <v>72</v>
       </c>
       <c r="F24" s="26" t="str">
@@ -26803,7 +27280,7 @@
       </c>
     </row>
     <row r="25" spans="3:18" x14ac:dyDescent="0.15">
-      <c r="E25" s="50" t="s">
+      <c r="E25" s="49" t="s">
         <v>73</v>
       </c>
       <c r="F25" s="29">
@@ -26849,7 +27326,7 @@
       <c r="Q25" s="42"/>
     </row>
     <row r="26" spans="3:18" x14ac:dyDescent="0.15">
-      <c r="E26" s="51" t="s">
+      <c r="E26" s="50" t="s">
         <v>74</v>
       </c>
       <c r="F26" s="32" t="str">
@@ -27030,7 +27507,7 @@
     </row>
     <row r="34" spans="5:18" x14ac:dyDescent="0.15">
       <c r="E34" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F34" s="24" t="s">
@@ -28039,7 +28516,7 @@
     </row>
     <row r="56" spans="3:18" ht="3" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="57" spans="3:18" x14ac:dyDescent="0.15">
-      <c r="E57" s="49" t="s">
+      <c r="E57" s="48" t="s">
         <v>114</v>
       </c>
       <c r="F57" s="26">
@@ -28246,7 +28723,7 @@
     </row>
     <row r="67" spans="5:20" x14ac:dyDescent="0.15">
       <c r="E67" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F67" s="24" t="s">
@@ -28501,7 +28978,7 @@
     </row>
     <row r="78" spans="5:20" x14ac:dyDescent="0.15">
       <c r="E78" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F78" s="37" t="s">
@@ -28884,7 +29361,7 @@
     </row>
     <row r="90" spans="3:20" x14ac:dyDescent="0.15">
       <c r="E90" s="10" t="str">
-        <f>+Input!$E$13</f>
+        <f>+Input!$E$14</f>
         <v>USDmn</v>
       </c>
       <c r="F90" s="37" t="s">

</xml_diff>